<commit_message>
finished queries and created html tables
</commit_message>
<xml_diff>
--- a/part3_queries.xlsx
+++ b/part3_queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emersonli/Documents/School/2023_2 Fall/Databases/Projects/Project 1/part3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1D512D-5601-504F-B1EF-32F5A3A59E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A453C4A2-31C2-2048-A276-0D84089A8930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{DD73E747-43A6-8745-B09B-0ED04D56C621}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>Pokemon</t>
   </si>
@@ -227,12 +227,6 @@
     <t>ItemID</t>
   </si>
   <si>
-    <t>Name (Pokemon)</t>
-  </si>
-  <si>
-    <t>Name (Item)</t>
-  </si>
-  <si>
     <t>Evolves_From</t>
   </si>
   <si>
@@ -240,6 +234,12 @@
   </si>
   <si>
     <t>Evolution Item</t>
+  </si>
+  <si>
+    <t>Held Item</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -599,21 +599,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED739181-3D0A-4E41-8B3C-0933D71D61C2}">
-  <dimension ref="A1:W51"/>
+  <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="15" max="15" width="13.33203125" customWidth="1"/>
     <col min="16" max="16" width="11.33203125" customWidth="1"/>
-    <col min="21" max="21" width="17.6640625" customWidth="1"/>
-    <col min="23" max="23" width="13.83203125" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="24" max="24" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -627,10 +628,10 @@
         <v>61</v>
       </c>
       <c r="N1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -662,10 +663,10 @@
         <v>62</v>
       </c>
       <c r="O2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R2" t="s">
         <v>1</v>
@@ -677,16 +678,19 @@
         <v>59</v>
       </c>
       <c r="U2" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="V2" t="s">
         <v>6</v>
       </c>
       <c r="W2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="X2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -714,17 +718,14 @@
       <c r="L3">
         <v>200</v>
       </c>
-      <c r="R3" t="s">
-        <v>7</v>
-      </c>
-      <c r="S3">
-        <v>318</v>
-      </c>
-      <c r="T3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W3" t="s">
+        <v>67</v>
+      </c>
+      <c r="X3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -752,17 +753,8 @@
       <c r="L4">
         <v>201</v>
       </c>
-      <c r="R4">
-        <v>2</v>
-      </c>
-      <c r="S4">
-        <v>405</v>
-      </c>
-      <c r="T4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -790,17 +782,8 @@
       <c r="L5">
         <v>400</v>
       </c>
-      <c r="R5">
-        <v>3</v>
-      </c>
-      <c r="S5">
-        <v>525</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -829,7 +812,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -858,7 +841,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -887,7 +870,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -916,7 +899,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -945,7 +928,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -974,7 +957,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1003,7 +986,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1032,7 +1015,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1061,7 +1044,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1090,7 +1073,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
added check to make sure money does not go negative
</commit_message>
<xml_diff>
--- a/part3_queries.xlsx
+++ b/part3_queries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emersonli/Documents/School/2023_2 Fall/Databases/Projects/Project 1/part3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E28A69-022F-A94A-AC8B-4DC152FF5A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6DB9A7-2BB3-1A4F-BABD-0062A0F036DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{DD73E747-43A6-8745-B09B-0ED04D56C621}"/>
+    <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{DD73E747-43A6-8745-B09B-0ED04D56C621}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -602,7 +602,7 @@
   <dimension ref="A1:X51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1389,12 +1389,8 @@
       <c r="F28">
         <v>325</v>
       </c>
-      <c r="H28" s="1">
-        <v>10</v>
-      </c>
-      <c r="I28" s="1">
-        <v>201</v>
-      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">

</xml_diff>